<commit_message>
suppression des colonnes commentaire et statut
</commit_message>
<xml_diff>
--- a/src/main/resources/template-export-convergence.xlsx
+++ b/src/main/resources/template-export-convergence.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cjuillard\Documents\segur\squash-convergence-export-plugin\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4C667C1-2613-4195-A0C7-B29A28090455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1ABB709-7583-4887-8F58-3BE32780270E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-6195" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33360" yWindow="-3480" windowWidth="17280" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exigences" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Profil</t>
   </si>
@@ -98,12 +98,6 @@
   </si>
   <si>
     <t>Exigence</t>
-  </si>
-  <si>
-    <t>Statut publication</t>
-  </si>
-  <si>
-    <t>Commentaire</t>
   </si>
   <si>
     <t>N° preuve</t>
@@ -584,11 +578,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Feuil5"/>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="D33" sqref="D33"/>
+      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.25" defaultRowHeight="15.6"/>
@@ -601,11 +595,11 @@
     <col min="6" max="6" width="18.58203125" style="4" customWidth="1"/>
     <col min="7" max="7" width="66.4140625" style="5" customWidth="1"/>
     <col min="8" max="8" width="18.58203125" style="6" customWidth="1"/>
-    <col min="9" max="11" width="30.58203125" style="5" customWidth="1"/>
-    <col min="12" max="16384" width="9.25" style="7"/>
+    <col min="9" max="9" width="30.58203125" style="5" customWidth="1"/>
+    <col min="10" max="16384" width="9.25" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="56.25" customHeight="1">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="56.25" customHeight="1">
       <c r="A1" s="8" t="s">
         <v>12</v>
       </c>
@@ -628,19 +622,13 @@
         <v>3</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="11" t="s">
-        <v>14</v>
-      </c>
     </row>
-    <row r="2" spans="1:11" s="18" customFormat="1" ht="68.25" customHeight="1">
+    <row r="2" spans="1:9" s="18" customFormat="1" ht="68.25" customHeight="1">
       <c r="A2" s="19" t="s">
         <v>7</v>
       </c>
@@ -668,8 +656,6 @@
       <c r="I2" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
     </row>
   </sheetData>
   <autoFilter ref="B1:I2" xr:uid="{00000000-0009-0000-0000-000000000000}"/>

</xml_diff>